<commit_message>
alteração do módulo de controle de contratos
</commit_message>
<xml_diff>
--- a/database/controle_processos.xlsx
+++ b/database/controle_processos.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -26,7 +25,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,10 +50,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -62,7 +75,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -427,11 +440,23 @@
   </sheetPr>
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="35" customWidth="1" min="4" max="4"/>
+    <col width="40" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -542,7 +567,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Sessão Pública</t>
+          <t>Em recurso</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -598,10 +623,9 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Sessão Pública</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr"/>
+          <t>Em recurso</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -650,10 +674,9 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Sessão Pública</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr"/>
+          <t>Em recurso</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -705,7 +728,6 @@
           <t>Sessão Pública</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -810,7 +832,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Edital</t>
+          <t>CJACM</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -1093,7 +1115,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1145,7 +1166,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1197,7 +1217,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1249,7 +1268,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1301,7 +1319,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1353,7 +1370,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1405,7 +1421,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1457,7 +1472,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1509,7 +1523,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1561,7 +1574,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1613,7 +1625,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1665,7 +1676,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1717,7 +1727,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1769,7 +1778,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1821,7 +1829,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1873,7 +1880,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1925,7 +1931,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1977,7 +1982,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2029,7 +2033,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2081,7 +2084,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2133,7 +2135,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2185,7 +2186,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2237,7 +2237,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2289,7 +2288,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2341,7 +2339,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2393,7 +2390,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2445,7 +2441,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2497,7 +2492,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2549,7 +2543,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2601,7 +2594,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2653,7 +2645,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2705,7 +2696,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2757,7 +2747,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2809,7 +2798,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2861,7 +2849,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2913,7 +2900,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2965,7 +2951,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3017,7 +3002,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3069,7 +3053,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3121,7 +3104,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -3173,7 +3155,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3225,7 +3206,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3277,7 +3257,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3329,7 +3308,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3381,7 +3359,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3433,7 +3410,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3485,7 +3461,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3537,7 +3512,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3589,7 +3563,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3641,7 +3614,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3693,7 +3665,6 @@
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3745,7 +3716,6 @@
           <t>Devolvido por Nota</t>
         </is>
       </c>
-      <c r="L63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3909,7 +3879,6 @@
           <t>Devolvido por Nota</t>
         </is>
       </c>
-      <c r="L66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -4353,7 +4322,6 @@
           <t>Setor Responsável</t>
         </is>
       </c>
-      <c r="L74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -4405,7 +4373,6 @@
           <t>Setor Responsável</t>
         </is>
       </c>
-      <c r="L75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4424,7 +4391,6 @@
           <t>62055.XXXXXX/2024-XX</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr"/>
       <c r="F76" t="n">
         <v>787000</v>
       </c>
@@ -4438,16 +4404,13 @@
           <t>Com7ºDN</t>
         </is>
       </c>
-      <c r="I76" t="inlineStr"/>
-      <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr">
         <is>
           <t>Planejamento</t>
         </is>
       </c>
-      <c r="L76" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
comit texto msg padrao
</commit_message>
<xml_diff>
--- a/database/controle_processos.xlsx
+++ b/database/controle_processos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="187">
   <si>
     <t>mod</t>
   </si>
@@ -55,15 +55,12 @@
     <t>PE</t>
   </si>
   <si>
-    <t>A</t>
+    <t>CC</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>DE</t>
   </si>
   <si>
@@ -253,9 +250,6 @@
     <t>62055.001299/2024-17</t>
   </si>
   <si>
-    <t>62055.013038/2023-69</t>
-  </si>
-  <si>
     <t>62055.XXXXXX/2024-XX</t>
   </si>
   <si>
@@ -433,9 +427,6 @@
     <t>Aquisição de mobiliário para nova sede da CFB</t>
   </si>
   <si>
-    <t>CC Construção da CFB</t>
-  </si>
-  <si>
     <t>Dispensa1</t>
   </si>
   <si>
@@ -538,9 +529,6 @@
     <t>ERMBRA</t>
   </si>
   <si>
-    <t>Eng</t>
-  </si>
-  <si>
     <t>ASD</t>
   </si>
   <si>
@@ -551,6 +539,9 @@
   </si>
   <si>
     <t>Sessão Pública</t>
+  </si>
+  <si>
+    <t>Nota Técnica</t>
   </si>
   <si>
     <t>CJACM</t>
@@ -941,7 +932,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L76"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -996,31 +987,31 @@
         <v>2023</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F2">
         <v>787010</v>
       </c>
       <c r="G2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="L2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1034,28 +1025,28 @@
         <v>2023</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F3">
         <v>787310</v>
       </c>
       <c r="G3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1069,28 +1060,28 @@
         <v>2023</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F4">
         <v>787000</v>
       </c>
       <c r="G4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1104,33 +1095,33 @@
         <v>2023</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F5">
         <v>787200</v>
       </c>
       <c r="G5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1139,31 +1130,31 @@
         <v>2024</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F6">
         <v>787200</v>
       </c>
       <c r="G6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J6" t="s">
+        <v>171</v>
+      </c>
+      <c r="K6" t="s">
         <v>175</v>
       </c>
-      <c r="K6" t="s">
-        <v>179</v>
-      </c>
       <c r="L6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1177,31 +1168,31 @@
         <v>2024</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F7">
         <v>787010</v>
       </c>
       <c r="G7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="L7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1215,31 +1206,31 @@
         <v>2024</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F8">
         <v>787000</v>
       </c>
       <c r="G8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="L8" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1253,31 +1244,31 @@
         <v>2024</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F9">
         <v>787000</v>
       </c>
       <c r="G9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J9" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="L9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1291,31 +1282,31 @@
         <v>2024</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F10">
         <v>787400</v>
       </c>
       <c r="G10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J10" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="L10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1329,31 +1320,31 @@
         <v>2024</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F11">
         <v>787000</v>
       </c>
       <c r="G11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I11" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J11" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="L11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1367,28 +1358,28 @@
         <v>2024</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F12">
         <v>787010</v>
       </c>
       <c r="G12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I12" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J12" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1402,28 +1393,28 @@
         <v>2024</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F13">
         <v>787200</v>
       </c>
       <c r="G13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J13" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1437,28 +1428,28 @@
         <v>2024</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F14">
         <v>787310</v>
       </c>
       <c r="G14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J14" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K14" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1472,28 +1463,28 @@
         <v>2024</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F15">
         <v>787000</v>
       </c>
       <c r="G15" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I15" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J15" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1507,28 +1498,28 @@
         <v>2024</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F16">
         <v>787320</v>
       </c>
       <c r="G16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J16" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K16" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1542,28 +1533,28 @@
         <v>2024</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F17">
         <v>787000</v>
       </c>
       <c r="G17" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H17" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I17" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J17" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K17" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1577,28 +1568,28 @@
         <v>2024</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F18">
         <v>787000</v>
       </c>
       <c r="G18" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J18" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K18" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1612,28 +1603,28 @@
         <v>2024</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F19">
         <v>787000</v>
       </c>
       <c r="G19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J19" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1647,28 +1638,28 @@
         <v>2024</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F20">
         <v>787000</v>
       </c>
       <c r="G20" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J20" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K20" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1682,28 +1673,28 @@
         <v>2024</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F21">
         <v>787000</v>
       </c>
       <c r="G21" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J21" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K21" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1717,28 +1708,28 @@
         <v>2024</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F22">
         <v>787000</v>
       </c>
       <c r="G22" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H22" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I22" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J22" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K22" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1752,28 +1743,28 @@
         <v>2024</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F23">
         <v>787000</v>
       </c>
       <c r="G23" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H23" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I23" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J23" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K23" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1787,28 +1778,28 @@
         <v>2024</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F24">
         <v>787400</v>
       </c>
       <c r="G24" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H24" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I24" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J24" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K24" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1822,28 +1813,28 @@
         <v>2024</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F25">
         <v>787000</v>
       </c>
       <c r="G25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J25" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K25" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1857,28 +1848,28 @@
         <v>2024</v>
       </c>
       <c r="D26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F26">
         <v>787000</v>
       </c>
       <c r="G26" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H26" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I26" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J26" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K26" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1892,28 +1883,28 @@
         <v>2024</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F27">
         <v>787000</v>
       </c>
       <c r="G27" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H27" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I27" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J27" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K27" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1927,28 +1918,28 @@
         <v>2024</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F28">
         <v>787010</v>
       </c>
       <c r="G28" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H28" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I28" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J28" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K28" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1962,28 +1953,28 @@
         <v>2024</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F29">
         <v>787200</v>
       </c>
       <c r="G29" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H29" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I29" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J29" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K29" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1997,28 +1988,28 @@
         <v>2024</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E30" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F30">
         <v>787900</v>
       </c>
       <c r="G30" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H30" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I30" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J30" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K30" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2032,28 +2023,28 @@
         <v>2024</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F31">
         <v>787000</v>
       </c>
       <c r="G31" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H31" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I31" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J31" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K31" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2067,28 +2058,28 @@
         <v>2024</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E32" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F32">
         <v>787000</v>
       </c>
       <c r="G32" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H32" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I32" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J32" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="K32" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -2102,28 +2093,28 @@
         <v>2024</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F33">
         <v>787010</v>
       </c>
       <c r="G33" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H33" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I33" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J33" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K33" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2137,28 +2128,28 @@
         <v>2024</v>
       </c>
       <c r="D34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F34">
         <v>787010</v>
       </c>
       <c r="G34" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H34" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I34" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J34" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K34" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2172,28 +2163,28 @@
         <v>2024</v>
       </c>
       <c r="D35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F35">
         <v>787010</v>
       </c>
       <c r="G35" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H35" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I35" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J35" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K35" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2207,28 +2198,28 @@
         <v>2024</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F36">
         <v>787010</v>
       </c>
       <c r="G36" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H36" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I36" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J36" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K36" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2242,28 +2233,28 @@
         <v>2024</v>
       </c>
       <c r="D37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F37">
         <v>787010</v>
       </c>
       <c r="G37" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H37" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I37" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J37" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K37" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2277,28 +2268,28 @@
         <v>2024</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F38">
         <v>787000</v>
       </c>
       <c r="G38" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H38" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I38" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J38" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K38" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -2312,28 +2303,28 @@
         <v>2024</v>
       </c>
       <c r="D39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F39">
         <v>787000</v>
       </c>
       <c r="G39" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H39" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I39" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J39" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K39" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2347,28 +2338,28 @@
         <v>2024</v>
       </c>
       <c r="D40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E40" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F40">
         <v>787320</v>
       </c>
       <c r="G40" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H40" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I40" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J40" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K40" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2382,28 +2373,28 @@
         <v>2024</v>
       </c>
       <c r="D41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E41" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F41">
         <v>787400</v>
       </c>
       <c r="G41" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H41" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I41" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J41" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K41" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2417,28 +2408,28 @@
         <v>2024</v>
       </c>
       <c r="D42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E42" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F42">
         <v>787000</v>
       </c>
       <c r="G42" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H42" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I42" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J42" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K42" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2452,28 +2443,28 @@
         <v>2024</v>
       </c>
       <c r="D43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F43">
         <v>787000</v>
       </c>
       <c r="G43" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H43" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I43" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J43" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K43" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2487,28 +2478,28 @@
         <v>2024</v>
       </c>
       <c r="D44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E44" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F44">
         <v>787010</v>
       </c>
       <c r="G44" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H44" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I44" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J44" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K44" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2522,28 +2513,28 @@
         <v>2024</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E45" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F45">
         <v>787000</v>
       </c>
       <c r="G45" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H45" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I45" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J45" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K45" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2557,28 +2548,28 @@
         <v>2024</v>
       </c>
       <c r="D46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E46" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F46">
         <v>787000</v>
       </c>
       <c r="G46" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H46" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I46" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J46" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K46" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2592,28 +2583,28 @@
         <v>2024</v>
       </c>
       <c r="D47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E47" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F47">
         <v>787000</v>
       </c>
       <c r="G47" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H47" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I47" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J47" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K47" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2627,31 +2618,31 @@
         <v>2024</v>
       </c>
       <c r="D48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E48" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F48">
         <v>787000</v>
       </c>
       <c r="G48" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H48" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I48" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J48" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K48" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -2662,31 +2653,31 @@
         <v>2024</v>
       </c>
       <c r="D49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E49" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F49">
         <v>787000</v>
       </c>
       <c r="G49" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H49" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I49" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J49" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K49" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -2697,31 +2688,31 @@
         <v>2024</v>
       </c>
       <c r="D50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E50" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F50">
         <v>787400</v>
       </c>
       <c r="G50" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H50" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I50" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J50" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K50" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -2732,31 +2723,31 @@
         <v>2024</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E51" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F51">
         <v>787000</v>
       </c>
       <c r="G51" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H51" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I51" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J51" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K51" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -2767,31 +2758,31 @@
         <v>2024</v>
       </c>
       <c r="D52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E52" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F52">
         <v>787320</v>
       </c>
       <c r="G52" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H52" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I52" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J52" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K52" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -2802,31 +2793,31 @@
         <v>2024</v>
       </c>
       <c r="D53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E53" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F53">
         <v>787320</v>
       </c>
       <c r="G53" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H53" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I53" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J53" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K53" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -2837,31 +2828,31 @@
         <v>2024</v>
       </c>
       <c r="D54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E54" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F54">
         <v>787010</v>
       </c>
       <c r="G54" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H54" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I54" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J54" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K54" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -2872,31 +2863,31 @@
         <v>2024</v>
       </c>
       <c r="D55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E55" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F55">
         <v>787000</v>
       </c>
       <c r="G55" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H55" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I55" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J55" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K55" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -2907,31 +2898,31 @@
         <v>2024</v>
       </c>
       <c r="D56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E56" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F56">
         <v>787000</v>
       </c>
       <c r="G56" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H56" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I56" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J56" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K56" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -2942,31 +2933,31 @@
         <v>2024</v>
       </c>
       <c r="D57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E57" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F57">
         <v>787000</v>
       </c>
       <c r="G57" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H57" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I57" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J57" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K57" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -2977,31 +2968,31 @@
         <v>2024</v>
       </c>
       <c r="D58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E58" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F58">
         <v>787400</v>
       </c>
       <c r="G58" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H58" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I58" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J58" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K58" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -3012,31 +3003,31 @@
         <v>2024</v>
       </c>
       <c r="D59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E59" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F59">
         <v>787200</v>
       </c>
       <c r="G59" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H59" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I59" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J59" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K59" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" t="s">
         <v>12</v>
       </c>
@@ -3047,31 +3038,31 @@
         <v>2024</v>
       </c>
       <c r="D60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E60" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F60">
         <v>787310</v>
       </c>
       <c r="G60" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H60" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I60" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J60" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K60" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -3082,31 +3073,31 @@
         <v>2024</v>
       </c>
       <c r="D61" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E61" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F61">
         <v>787320</v>
       </c>
       <c r="G61" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H61" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I61" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J61" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K61" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -3117,31 +3108,31 @@
         <v>2024</v>
       </c>
       <c r="D62" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E62" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F62">
         <v>787010</v>
       </c>
       <c r="G62" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H62" t="s">
+        <v>153</v>
+      </c>
+      <c r="I62" t="s">
         <v>156</v>
       </c>
-      <c r="I62" t="s">
-        <v>159</v>
-      </c>
       <c r="J62" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K62" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -3152,139 +3143,139 @@
         <v>2024</v>
       </c>
       <c r="D63" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E63" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F63">
         <v>787010</v>
       </c>
       <c r="G63" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H63" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I63" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J63" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K63" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C64">
         <v>2024</v>
       </c>
       <c r="D64" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E64" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F64">
-        <v>787000</v>
+        <v>787010</v>
       </c>
       <c r="G64" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="H64" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I64" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="J64" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K64" t="s">
         <v>179</v>
       </c>
-      <c r="L64" t="s">
-        <v>187</v>
-      </c>
     </row>
     <row r="65" spans="1:12">
       <c r="A65" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="D65" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="E65" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F65">
-        <v>787000</v>
+        <v>787010</v>
       </c>
       <c r="G65" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H65" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I65" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="J65" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K65" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L65" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B66">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="C66">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="D66" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="E66" t="s">
         <v>138</v>
       </c>
       <c r="F66">
-        <v>787010</v>
+        <v>787310</v>
       </c>
       <c r="G66" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H66" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I66" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J66" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K66" t="s">
-        <v>182</v>
+        <v>180</v>
+      </c>
+      <c r="L66" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -3292,13 +3283,13 @@
         <v>15</v>
       </c>
       <c r="B67">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C67">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="D67" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="E67" t="s">
         <v>139</v>
@@ -3307,36 +3298,36 @@
         <v>787000</v>
       </c>
       <c r="G67" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H67" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I67" t="s">
+        <v>162</v>
+      </c>
+      <c r="J67" t="s">
+        <v>171</v>
+      </c>
+      <c r="K67" t="s">
         <v>174</v>
       </c>
-      <c r="J67" t="s">
-        <v>175</v>
-      </c>
-      <c r="K67" t="s">
-        <v>179</v>
-      </c>
       <c r="L67" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" spans="1:12">
       <c r="A68" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C68">
         <v>2023</v>
       </c>
       <c r="D68" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E68" t="s">
         <v>140</v>
@@ -3345,308 +3336,194 @@
         <v>787010</v>
       </c>
       <c r="G68" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="H68" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="I68" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="J68" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K68" t="s">
+        <v>174</v>
+      </c>
+      <c r="L68" t="s">
         <v>183</v>
-      </c>
-      <c r="L68" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:12">
       <c r="A69" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B69">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C69">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D69" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E69" t="s">
         <v>141</v>
       </c>
       <c r="F69">
-        <v>787310</v>
+        <v>787200</v>
       </c>
       <c r="G69" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H69" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I69" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J69" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K69" t="s">
+        <v>181</v>
+      </c>
+      <c r="L69" t="s">
         <v>183</v>
-      </c>
-      <c r="L69" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:12">
       <c r="A70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B70">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C70">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D70" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E70" t="s">
         <v>142</v>
       </c>
       <c r="F70">
-        <v>787000</v>
+        <v>787010</v>
       </c>
       <c r="G70" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H70" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I70" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J70" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K70" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="L70" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="71" spans="1:12">
       <c r="A71" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B71">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C71">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D71" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E71" t="s">
         <v>143</v>
       </c>
       <c r="F71">
-        <v>787010</v>
+        <v>787000</v>
       </c>
       <c r="G71" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H71" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I71" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J71" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K71" t="s">
-        <v>178</v>
-      </c>
-      <c r="L71" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="72" spans="1:12">
       <c r="A72" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B72">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C72">
         <v>2024</v>
       </c>
       <c r="D72" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E72" t="s">
         <v>144</v>
       </c>
       <c r="F72">
-        <v>787200</v>
+        <v>787000</v>
       </c>
       <c r="G72" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H72" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I72" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="J72" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K72" t="s">
-        <v>184</v>
-      </c>
-      <c r="L72" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="73" spans="1:12">
       <c r="A73" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B73">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="C73">
         <v>2024</v>
       </c>
       <c r="D73" t="s">
-        <v>22</v>
-      </c>
-      <c r="E73" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="F73">
-        <v>787010</v>
+        <v>787000</v>
       </c>
       <c r="G73" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H73" t="s">
-        <v>160</v>
-      </c>
-      <c r="I73" t="s">
-        <v>166</v>
-      </c>
-      <c r="J73" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="K73" t="s">
-        <v>185</v>
-      </c>
-      <c r="L73" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12">
-      <c r="A74" t="s">
-        <v>16</v>
-      </c>
-      <c r="B74">
-        <v>7</v>
-      </c>
-      <c r="C74">
-        <v>2024</v>
-      </c>
-      <c r="D74" t="s">
-        <v>23</v>
-      </c>
-      <c r="E74" t="s">
-        <v>146</v>
-      </c>
-      <c r="F74">
-        <v>787000</v>
-      </c>
-      <c r="G74" t="s">
-        <v>150</v>
-      </c>
-      <c r="H74" t="s">
-        <v>158</v>
-      </c>
-      <c r="I74" t="s">
-        <v>165</v>
-      </c>
-      <c r="J74" t="s">
-        <v>175</v>
-      </c>
-      <c r="K74" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12">
-      <c r="A75" t="s">
-        <v>16</v>
-      </c>
-      <c r="B75">
-        <v>8</v>
-      </c>
-      <c r="C75">
-        <v>2024</v>
-      </c>
-      <c r="D75" t="s">
-        <v>24</v>
-      </c>
-      <c r="E75" t="s">
-        <v>147</v>
-      </c>
-      <c r="F75">
-        <v>787000</v>
-      </c>
-      <c r="G75" t="s">
-        <v>150</v>
-      </c>
-      <c r="H75" t="s">
-        <v>158</v>
-      </c>
-      <c r="I75" t="s">
-        <v>167</v>
-      </c>
-      <c r="J75" t="s">
-        <v>175</v>
-      </c>
-      <c r="K75" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12">
-      <c r="A76" t="s">
-        <v>12</v>
-      </c>
-      <c r="B76">
-        <v>59</v>
-      </c>
-      <c r="C76">
-        <v>2024</v>
-      </c>
-      <c r="D76" t="s">
-        <v>80</v>
-      </c>
-      <c r="F76">
-        <v>787000</v>
-      </c>
-      <c r="G76" t="s">
-        <v>150</v>
-      </c>
-      <c r="H76" t="s">
-        <v>158</v>
-      </c>
-      <c r="K76" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizacao do painel de contratos
</commit_message>
<xml_diff>
--- a/database/controle_processos.xlsx
+++ b/database/controle_processos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="194">
   <si>
     <t>mod</t>
   </si>
@@ -451,6 +451,27 @@
     <t>Dispensa8</t>
   </si>
   <si>
+    <t>787010</t>
+  </si>
+  <si>
+    <t>787310</t>
+  </si>
+  <si>
+    <t>787000</t>
+  </si>
+  <si>
+    <t>787200</t>
+  </si>
+  <si>
+    <t>787400</t>
+  </si>
+  <si>
+    <t>787320</t>
+  </si>
+  <si>
+    <t>787900</t>
+  </si>
+  <si>
     <t>CENTRO DE INTENDÊNCIA DA MARINHA EM BRASÍLIA</t>
   </si>
   <si>
@@ -463,15 +484,15 @@
     <t>GRUPAMENTO DE FUZILEIROS NAVAIS DE BRASÍLIA</t>
   </si>
   <si>
+    <t>ESTAÇÃO RÁDIO DA MARINHA EM BRASÍLIA</t>
+  </si>
+  <si>
+    <t>CAPITANIA FLUVIAL DE BRASÍLIA</t>
+  </si>
+  <si>
     <t>NÚCLEO DE IMPLANTAÇÃO DO CENTRO DE INTENDÊNCIA DA MARINHA EM BRASÍLIA</t>
   </si>
   <si>
-    <t>ESTAÇÃO RÁDIO DA MARINHA EM BRASÍLIA</t>
-  </si>
-  <si>
-    <t>CAPITANIA FLUVIAL DE BRASÍLIA</t>
-  </si>
-  <si>
     <t>CENTRO DE INSTRUÇÃO E ADESTRAMENTO DE BRASÍLIA</t>
   </si>
   <si>
@@ -487,13 +508,13 @@
     <t>GptFNB</t>
   </si>
   <si>
+    <t>ERMB</t>
+  </si>
+  <si>
+    <t>CFB</t>
+  </si>
+  <si>
     <t>NI-CeIMBra</t>
-  </si>
-  <si>
-    <t>ERMB</t>
-  </si>
-  <si>
-    <t>CFB</t>
   </si>
   <si>
     <t>CIAB</t>
@@ -992,26 +1013,26 @@
       <c r="E2" t="s">
         <v>79</v>
       </c>
-      <c r="F2">
-        <v>787010</v>
+      <c r="F2" t="s">
+        <v>145</v>
       </c>
       <c r="G2" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="H2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="I2" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="J2" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K2" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="L2" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1030,23 +1051,23 @@
       <c r="E3" t="s">
         <v>80</v>
       </c>
-      <c r="F3">
-        <v>787310</v>
+      <c r="F3" t="s">
+        <v>146</v>
       </c>
       <c r="G3" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="H3" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="I3" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="J3" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K3" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1065,23 +1086,23 @@
       <c r="E4" t="s">
         <v>81</v>
       </c>
-      <c r="F4">
-        <v>787000</v>
+      <c r="F4" t="s">
+        <v>147</v>
       </c>
       <c r="G4" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H4" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I4" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="J4" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K4" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1100,23 +1121,23 @@
       <c r="E5" t="s">
         <v>82</v>
       </c>
-      <c r="F5">
-        <v>787200</v>
+      <c r="F5" t="s">
+        <v>148</v>
       </c>
       <c r="G5" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="H5" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="I5" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="J5" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K5" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1135,26 +1156,26 @@
       <c r="E6" t="s">
         <v>83</v>
       </c>
-      <c r="F6">
-        <v>787200</v>
+      <c r="F6" t="s">
+        <v>148</v>
       </c>
       <c r="G6" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="H6" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="I6" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="J6" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K6" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="L6" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1173,26 +1194,26 @@
       <c r="E7" t="s">
         <v>84</v>
       </c>
-      <c r="F7">
-        <v>787010</v>
+      <c r="F7" t="s">
+        <v>145</v>
       </c>
       <c r="G7" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="H7" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="I7" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="J7" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K7" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="L7" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1211,26 +1232,26 @@
       <c r="E8" t="s">
         <v>85</v>
       </c>
-      <c r="F8">
-        <v>787000</v>
+      <c r="F8" t="s">
+        <v>147</v>
       </c>
       <c r="G8" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H8" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I8" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="J8" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K8" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="L8" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1249,26 +1270,26 @@
       <c r="E9" t="s">
         <v>86</v>
       </c>
-      <c r="F9">
-        <v>787000</v>
+      <c r="F9" t="s">
+        <v>147</v>
       </c>
       <c r="G9" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H9" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I9" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="J9" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K9" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="L9" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1287,26 +1308,26 @@
       <c r="E10" t="s">
         <v>87</v>
       </c>
-      <c r="F10">
-        <v>787400</v>
+      <c r="F10" t="s">
+        <v>149</v>
       </c>
       <c r="G10" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="H10" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="I10" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="J10" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K10" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="L10" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1325,26 +1346,26 @@
       <c r="E11" t="s">
         <v>88</v>
       </c>
-      <c r="F11">
-        <v>787000</v>
+      <c r="F11" t="s">
+        <v>147</v>
       </c>
       <c r="G11" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H11" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I11" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="J11" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K11" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="L11" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1363,23 +1384,23 @@
       <c r="E12" t="s">
         <v>89</v>
       </c>
-      <c r="F12">
-        <v>787010</v>
+      <c r="F12" t="s">
+        <v>145</v>
       </c>
       <c r="G12" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="H12" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="I12" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="J12" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K12" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1398,23 +1419,23 @@
       <c r="E13" t="s">
         <v>90</v>
       </c>
-      <c r="F13">
-        <v>787200</v>
+      <c r="F13" t="s">
+        <v>148</v>
       </c>
       <c r="G13" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="H13" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="I13" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="J13" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K13" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1433,23 +1454,23 @@
       <c r="E14" t="s">
         <v>91</v>
       </c>
-      <c r="F14">
-        <v>787310</v>
+      <c r="F14" t="s">
+        <v>146</v>
       </c>
       <c r="G14" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="H14" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="I14" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="J14" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K14" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1468,23 +1489,23 @@
       <c r="E15" t="s">
         <v>92</v>
       </c>
-      <c r="F15">
-        <v>787000</v>
+      <c r="F15" t="s">
+        <v>147</v>
       </c>
       <c r="G15" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H15" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I15" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="J15" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K15" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1503,23 +1524,23 @@
       <c r="E16" t="s">
         <v>93</v>
       </c>
-      <c r="F16">
-        <v>787320</v>
+      <c r="F16" t="s">
+        <v>150</v>
       </c>
       <c r="G16" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="H16" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="I16" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="J16" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K16" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1538,23 +1559,23 @@
       <c r="E17" t="s">
         <v>94</v>
       </c>
-      <c r="F17">
-        <v>787000</v>
+      <c r="F17" t="s">
+        <v>147</v>
       </c>
       <c r="G17" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H17" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I17" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J17" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K17" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1573,23 +1594,23 @@
       <c r="E18" t="s">
         <v>95</v>
       </c>
-      <c r="F18">
-        <v>787000</v>
+      <c r="F18" t="s">
+        <v>147</v>
       </c>
       <c r="G18" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H18" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I18" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J18" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K18" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1608,23 +1629,23 @@
       <c r="E19" t="s">
         <v>96</v>
       </c>
-      <c r="F19">
-        <v>787000</v>
+      <c r="F19" t="s">
+        <v>147</v>
       </c>
       <c r="G19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H19" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I19" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J19" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K19" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1643,23 +1664,23 @@
       <c r="E20" t="s">
         <v>97</v>
       </c>
-      <c r="F20">
-        <v>787000</v>
+      <c r="F20" t="s">
+        <v>147</v>
       </c>
       <c r="G20" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H20" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I20" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J20" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K20" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1678,23 +1699,23 @@
       <c r="E21" t="s">
         <v>98</v>
       </c>
-      <c r="F21">
-        <v>787000</v>
+      <c r="F21" t="s">
+        <v>147</v>
       </c>
       <c r="G21" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H21" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I21" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J21" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K21" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1713,23 +1734,23 @@
       <c r="E22" t="s">
         <v>99</v>
       </c>
-      <c r="F22">
-        <v>787000</v>
+      <c r="F22" t="s">
+        <v>147</v>
       </c>
       <c r="G22" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H22" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I22" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J22" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K22" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1748,23 +1769,23 @@
       <c r="E23" t="s">
         <v>100</v>
       </c>
-      <c r="F23">
-        <v>787000</v>
+      <c r="F23" t="s">
+        <v>147</v>
       </c>
       <c r="G23" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H23" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I23" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J23" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K23" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1783,23 +1804,23 @@
       <c r="E24" t="s">
         <v>101</v>
       </c>
-      <c r="F24">
-        <v>787400</v>
+      <c r="F24" t="s">
+        <v>149</v>
       </c>
       <c r="G24" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="H24" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="I24" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="J24" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K24" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1818,23 +1839,23 @@
       <c r="E25" t="s">
         <v>102</v>
       </c>
-      <c r="F25">
-        <v>787000</v>
+      <c r="F25" t="s">
+        <v>147</v>
       </c>
       <c r="G25" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H25" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I25" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J25" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K25" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1853,23 +1874,23 @@
       <c r="E26" t="s">
         <v>103</v>
       </c>
-      <c r="F26">
-        <v>787000</v>
+      <c r="F26" t="s">
+        <v>147</v>
       </c>
       <c r="G26" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H26" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I26" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J26" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K26" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1888,23 +1909,23 @@
       <c r="E27" t="s">
         <v>86</v>
       </c>
-      <c r="F27">
-        <v>787000</v>
+      <c r="F27" t="s">
+        <v>147</v>
       </c>
       <c r="G27" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H27" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I27" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J27" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K27" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1923,23 +1944,23 @@
       <c r="E28" t="s">
         <v>90</v>
       </c>
-      <c r="F28">
-        <v>787010</v>
+      <c r="F28" t="s">
+        <v>145</v>
       </c>
       <c r="G28" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="H28" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="I28" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="J28" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K28" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1958,23 +1979,23 @@
       <c r="E29" t="s">
         <v>104</v>
       </c>
-      <c r="F29">
-        <v>787200</v>
+      <c r="F29" t="s">
+        <v>148</v>
       </c>
       <c r="G29" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="H29" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="I29" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="J29" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K29" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1993,23 +2014,23 @@
       <c r="E30" t="s">
         <v>105</v>
       </c>
-      <c r="F30">
-        <v>787900</v>
+      <c r="F30" t="s">
+        <v>151</v>
       </c>
       <c r="G30" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="H30" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="I30" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="J30" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K30" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2028,23 +2049,23 @@
       <c r="E31" t="s">
         <v>106</v>
       </c>
-      <c r="F31">
-        <v>787000</v>
+      <c r="F31" t="s">
+        <v>147</v>
       </c>
       <c r="G31" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H31" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I31" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J31" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K31" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2063,23 +2084,23 @@
       <c r="E32" t="s">
         <v>107</v>
       </c>
-      <c r="F32">
-        <v>787000</v>
+      <c r="F32" t="s">
+        <v>147</v>
       </c>
       <c r="G32" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H32" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I32" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J32" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="K32" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -2098,23 +2119,23 @@
       <c r="E33" t="s">
         <v>108</v>
       </c>
-      <c r="F33">
-        <v>787010</v>
+      <c r="F33" t="s">
+        <v>145</v>
       </c>
       <c r="G33" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="H33" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="I33" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="J33" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K33" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2133,23 +2154,23 @@
       <c r="E34" t="s">
         <v>109</v>
       </c>
-      <c r="F34">
-        <v>787010</v>
+      <c r="F34" t="s">
+        <v>145</v>
       </c>
       <c r="G34" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="H34" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="I34" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="J34" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K34" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2168,23 +2189,23 @@
       <c r="E35" t="s">
         <v>110</v>
       </c>
-      <c r="F35">
-        <v>787010</v>
+      <c r="F35" t="s">
+        <v>145</v>
       </c>
       <c r="G35" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="H35" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="I35" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="J35" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K35" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2203,23 +2224,23 @@
       <c r="E36" t="s">
         <v>111</v>
       </c>
-      <c r="F36">
-        <v>787010</v>
+      <c r="F36" t="s">
+        <v>145</v>
       </c>
       <c r="G36" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="H36" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="I36" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="J36" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K36" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2238,23 +2259,23 @@
       <c r="E37" t="s">
         <v>112</v>
       </c>
-      <c r="F37">
-        <v>787010</v>
+      <c r="F37" t="s">
+        <v>145</v>
       </c>
       <c r="G37" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="H37" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="I37" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J37" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K37" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2273,23 +2294,23 @@
       <c r="E38" t="s">
         <v>113</v>
       </c>
-      <c r="F38">
-        <v>787000</v>
+      <c r="F38" t="s">
+        <v>147</v>
       </c>
       <c r="G38" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H38" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I38" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J38" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K38" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -2308,23 +2329,23 @@
       <c r="E39" t="s">
         <v>114</v>
       </c>
-      <c r="F39">
-        <v>787000</v>
+      <c r="F39" t="s">
+        <v>147</v>
       </c>
       <c r="G39" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H39" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I39" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J39" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K39" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2343,23 +2364,23 @@
       <c r="E40" t="s">
         <v>115</v>
       </c>
-      <c r="F40">
-        <v>787320</v>
+      <c r="F40" t="s">
+        <v>150</v>
       </c>
       <c r="G40" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="H40" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="I40" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="J40" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K40" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2378,23 +2399,23 @@
       <c r="E41" t="s">
         <v>116</v>
       </c>
-      <c r="F41">
-        <v>787400</v>
+      <c r="F41" t="s">
+        <v>149</v>
       </c>
       <c r="G41" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="H41" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="I41" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="J41" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K41" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2413,23 +2434,23 @@
       <c r="E42" t="s">
         <v>117</v>
       </c>
-      <c r="F42">
-        <v>787000</v>
+      <c r="F42" t="s">
+        <v>147</v>
       </c>
       <c r="G42" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H42" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I42" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J42" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K42" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2448,23 +2469,23 @@
       <c r="E43" t="s">
         <v>82</v>
       </c>
-      <c r="F43">
-        <v>787000</v>
+      <c r="F43" t="s">
+        <v>147</v>
       </c>
       <c r="G43" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H43" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I43" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="J43" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K43" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2483,23 +2504,23 @@
       <c r="E44" t="s">
         <v>83</v>
       </c>
-      <c r="F44">
-        <v>787010</v>
+      <c r="F44" t="s">
+        <v>145</v>
       </c>
       <c r="G44" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="H44" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="I44" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="J44" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K44" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2518,23 +2539,23 @@
       <c r="E45" t="s">
         <v>118</v>
       </c>
-      <c r="F45">
-        <v>787000</v>
+      <c r="F45" t="s">
+        <v>147</v>
       </c>
       <c r="G45" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H45" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I45" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="J45" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K45" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2553,23 +2574,23 @@
       <c r="E46" t="s">
         <v>119</v>
       </c>
-      <c r="F46">
-        <v>787000</v>
+      <c r="F46" t="s">
+        <v>147</v>
       </c>
       <c r="G46" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H46" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I46" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="J46" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K46" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2588,23 +2609,23 @@
       <c r="E47" t="s">
         <v>120</v>
       </c>
-      <c r="F47">
-        <v>787000</v>
+      <c r="F47" t="s">
+        <v>147</v>
       </c>
       <c r="G47" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H47" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I47" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="J47" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K47" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2623,23 +2644,23 @@
       <c r="E48" t="s">
         <v>121</v>
       </c>
-      <c r="F48">
-        <v>787000</v>
+      <c r="F48" t="s">
+        <v>147</v>
       </c>
       <c r="G48" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H48" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I48" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="J48" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K48" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2658,23 +2679,23 @@
       <c r="E49" t="s">
         <v>122</v>
       </c>
-      <c r="F49">
-        <v>787000</v>
+      <c r="F49" t="s">
+        <v>147</v>
       </c>
       <c r="G49" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H49" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I49" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="J49" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K49" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2693,23 +2714,23 @@
       <c r="E50" t="s">
         <v>123</v>
       </c>
-      <c r="F50">
-        <v>787400</v>
+      <c r="F50" t="s">
+        <v>149</v>
       </c>
       <c r="G50" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="H50" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="I50" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="J50" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K50" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2728,23 +2749,23 @@
       <c r="E51" t="s">
         <v>124</v>
       </c>
-      <c r="F51">
-        <v>787000</v>
+      <c r="F51" t="s">
+        <v>147</v>
       </c>
       <c r="G51" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H51" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I51" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="J51" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K51" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2763,23 +2784,23 @@
       <c r="E52" t="s">
         <v>125</v>
       </c>
-      <c r="F52">
-        <v>787320</v>
+      <c r="F52" t="s">
+        <v>150</v>
       </c>
       <c r="G52" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="H52" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="I52" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="J52" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K52" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2798,23 +2819,23 @@
       <c r="E53" t="s">
         <v>126</v>
       </c>
-      <c r="F53">
-        <v>787320</v>
+      <c r="F53" t="s">
+        <v>150</v>
       </c>
       <c r="G53" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="H53" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="I53" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="J53" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K53" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2833,23 +2854,23 @@
       <c r="E54" t="s">
         <v>127</v>
       </c>
-      <c r="F54">
-        <v>787010</v>
+      <c r="F54" t="s">
+        <v>145</v>
       </c>
       <c r="G54" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="H54" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="I54" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="J54" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K54" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -2868,23 +2889,23 @@
       <c r="E55" t="s">
         <v>128</v>
       </c>
-      <c r="F55">
-        <v>787000</v>
+      <c r="F55" t="s">
+        <v>147</v>
       </c>
       <c r="G55" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H55" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I55" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="J55" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K55" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -2903,23 +2924,23 @@
       <c r="E56" t="s">
         <v>129</v>
       </c>
-      <c r="F56">
-        <v>787000</v>
+      <c r="F56" t="s">
+        <v>147</v>
       </c>
       <c r="G56" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H56" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I56" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="J56" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K56" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -2938,23 +2959,23 @@
       <c r="E57" t="s">
         <v>130</v>
       </c>
-      <c r="F57">
-        <v>787000</v>
+      <c r="F57" t="s">
+        <v>147</v>
       </c>
       <c r="G57" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H57" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I57" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="J57" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K57" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -2973,23 +2994,23 @@
       <c r="E58" t="s">
         <v>131</v>
       </c>
-      <c r="F58">
-        <v>787400</v>
+      <c r="F58" t="s">
+        <v>149</v>
       </c>
       <c r="G58" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="H58" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="I58" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="J58" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K58" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -3008,23 +3029,23 @@
       <c r="E59" t="s">
         <v>132</v>
       </c>
-      <c r="F59">
-        <v>787200</v>
+      <c r="F59" t="s">
+        <v>148</v>
       </c>
       <c r="G59" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="H59" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="I59" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="J59" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K59" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -3043,23 +3064,23 @@
       <c r="E60" t="s">
         <v>133</v>
       </c>
-      <c r="F60">
-        <v>787310</v>
+      <c r="F60" t="s">
+        <v>146</v>
       </c>
       <c r="G60" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="H60" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="I60" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="J60" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K60" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -3078,23 +3099,23 @@
       <c r="E61" t="s">
         <v>134</v>
       </c>
-      <c r="F61">
-        <v>787320</v>
+      <c r="F61" t="s">
+        <v>150</v>
       </c>
       <c r="G61" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="H61" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="I61" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="J61" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K61" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -3113,23 +3134,23 @@
       <c r="E62" t="s">
         <v>135</v>
       </c>
-      <c r="F62">
-        <v>787010</v>
+      <c r="F62" t="s">
+        <v>145</v>
       </c>
       <c r="G62" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="H62" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="I62" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="J62" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K62" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -3148,23 +3169,23 @@
       <c r="E63" t="s">
         <v>136</v>
       </c>
-      <c r="F63">
-        <v>787010</v>
+      <c r="F63" t="s">
+        <v>145</v>
       </c>
       <c r="G63" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="H63" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="I63" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="J63" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K63" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -3183,23 +3204,23 @@
       <c r="E64" t="s">
         <v>136</v>
       </c>
-      <c r="F64">
-        <v>787010</v>
+      <c r="F64" t="s">
+        <v>145</v>
       </c>
       <c r="G64" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="H64" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="I64" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="J64" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K64" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -3218,26 +3239,26 @@
       <c r="E65" t="s">
         <v>137</v>
       </c>
-      <c r="F65">
-        <v>787010</v>
+      <c r="F65" t="s">
+        <v>145</v>
       </c>
       <c r="G65" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="H65" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="I65" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="J65" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K65" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="L65" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -3256,26 +3277,26 @@
       <c r="E66" t="s">
         <v>138</v>
       </c>
-      <c r="F66">
-        <v>787310</v>
+      <c r="F66" t="s">
+        <v>146</v>
       </c>
       <c r="G66" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="H66" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="I66" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="J66" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K66" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="L66" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -3294,26 +3315,26 @@
       <c r="E67" t="s">
         <v>139</v>
       </c>
-      <c r="F67">
-        <v>787000</v>
+      <c r="F67" t="s">
+        <v>147</v>
       </c>
       <c r="G67" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H67" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I67" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="J67" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K67" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="L67" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -3332,26 +3353,26 @@
       <c r="E68" t="s">
         <v>140</v>
       </c>
-      <c r="F68">
-        <v>787010</v>
+      <c r="F68" t="s">
+        <v>145</v>
       </c>
       <c r="G68" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="H68" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="I68" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="J68" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K68" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="L68" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -3370,26 +3391,26 @@
       <c r="E69" t="s">
         <v>141</v>
       </c>
-      <c r="F69">
-        <v>787200</v>
+      <c r="F69" t="s">
+        <v>148</v>
       </c>
       <c r="G69" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="H69" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="I69" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="J69" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K69" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="L69" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -3408,26 +3429,26 @@
       <c r="E70" t="s">
         <v>142</v>
       </c>
-      <c r="F70">
-        <v>787010</v>
+      <c r="F70" t="s">
+        <v>145</v>
       </c>
       <c r="G70" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="H70" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="I70" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="J70" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K70" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="L70" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -3446,23 +3467,23 @@
       <c r="E71" t="s">
         <v>143</v>
       </c>
-      <c r="F71">
-        <v>787000</v>
+      <c r="F71" t="s">
+        <v>145</v>
       </c>
       <c r="G71" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="H71" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="I71" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="J71" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K71" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -3481,23 +3502,23 @@
       <c r="E72" t="s">
         <v>144</v>
       </c>
-      <c r="F72">
-        <v>787000</v>
+      <c r="F72" t="s">
+        <v>147</v>
       </c>
       <c r="G72" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H72" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I72" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="J72" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="K72" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -3513,17 +3534,17 @@
       <c r="D73" t="s">
         <v>78</v>
       </c>
-      <c r="F73">
-        <v>787000</v>
+      <c r="F73" t="s">
+        <v>147</v>
       </c>
       <c r="G73" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H73" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K73" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualização do controle de processos
</commit_message>
<xml_diff>
--- a/database/controle_processos.xlsx
+++ b/database/controle_processos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="105">
   <si>
     <t>mod</t>
   </si>
@@ -67,9 +67,6 @@
     <t>TJDL</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>62055.000344/2023-35</t>
   </si>
   <si>
@@ -157,7 +154,7 @@
     <t>Material de Pintura</t>
   </si>
   <si>
-    <t xml:space="preserve">Gás Liquefeito de Petróleo (GLP) </t>
+    <t>Nova Sede da CFB</t>
   </si>
   <si>
     <t>Transporte de Carga</t>
@@ -241,36 +238,21 @@
     <t>Dispensa8</t>
   </si>
   <si>
-    <t>787010</t>
-  </si>
-  <si>
-    <t>787310</t>
-  </si>
-  <si>
-    <t>787000</t>
-  </si>
-  <si>
-    <t>787200</t>
-  </si>
-  <si>
-    <t>787400</t>
-  </si>
-  <si>
-    <t>787320</t>
+    <t>COMANDO DO 7º DISTRITO NAVAL</t>
+  </si>
+  <si>
+    <t>CAPITANIA FLUVIAL DE ARAGUAIA-TOCANTINS</t>
+  </si>
+  <si>
+    <t>GRUPAMENTO DE FUZILEIROS NAVAIS DE BRASÍLIA</t>
+  </si>
+  <si>
+    <t>CENTRO DE INSTRUÇÃO E ADESTRAMENTO DE BRASÍLIA</t>
   </si>
   <si>
     <t>CENTRO DE INTENDÊNCIA DA MARINHA EM BRASÍLIA</t>
   </si>
   <si>
-    <t>CAPITANIA FLUVIAL DE ARAGUAIA-TOCANTINS</t>
-  </si>
-  <si>
-    <t>COMANDO DO 7º DISTRITO NAVAL</t>
-  </si>
-  <si>
-    <t>GRUPAMENTO DE FUZILEIROS NAVAIS DE BRASÍLIA</t>
-  </si>
-  <si>
     <t>ESTAÇÃO RÁDIO DA MARINHA EM BRASÍLIA</t>
   </si>
   <si>
@@ -280,18 +262,21 @@
     <t>NÚCLEO DE IMPLANTAÇÃO DO CENTRO DE INTENDÊNCIA DA MARINHA EM BRASÍLIA</t>
   </si>
   <si>
+    <t>Com7ºDN</t>
+  </si>
+  <si>
+    <t>CFAT</t>
+  </si>
+  <si>
+    <t>GptFNB</t>
+  </si>
+  <si>
+    <t>CIAB</t>
+  </si>
+  <si>
     <t>CeIMBra</t>
   </si>
   <si>
-    <t>CFAT</t>
-  </si>
-  <si>
-    <t>Com7ºDN</t>
-  </si>
-  <si>
-    <t>GptFNB</t>
-  </si>
-  <si>
     <t>ERMB</t>
   </si>
   <si>
@@ -331,16 +316,19 @@
     <t>Homologado</t>
   </si>
   <si>
+    <t>Em recurso</t>
+  </si>
+  <si>
+    <t>Setor Responsável</t>
+  </si>
+  <si>
+    <t>Edital</t>
+  </si>
+  <si>
+    <t>Planejamento</t>
+  </si>
+  <si>
     <t>Recomendações AGU</t>
-  </si>
-  <si>
-    <t>Planejamento</t>
-  </si>
-  <si>
-    <t>Setor Responsável</t>
-  </si>
-  <si>
-    <t>Concluído</t>
   </si>
 </sst>
 </file>
@@ -698,7 +686,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -753,28 +741,28 @@
         <v>2023</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" t="s">
-        <v>75</v>
+        <v>42</v>
+      </c>
+      <c r="F2">
+        <v>787000</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="I2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="J2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -788,28 +776,28 @@
         <v>2023</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" t="s">
-        <v>76</v>
+        <v>43</v>
+      </c>
+      <c r="F3">
+        <v>787310</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="J3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -823,28 +811,28 @@
         <v>2023</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" t="s">
-        <v>77</v>
+        <v>44</v>
+      </c>
+      <c r="F4">
+        <v>787000</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -858,28 +846,28 @@
         <v>2023</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" t="s">
-        <v>78</v>
+        <v>45</v>
+      </c>
+      <c r="F5">
+        <v>787200</v>
       </c>
       <c r="G5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" t="s">
         <v>84</v>
       </c>
-      <c r="H5" t="s">
-        <v>91</v>
-      </c>
       <c r="I5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="J5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -893,28 +881,28 @@
         <v>2024</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>78</v>
+        <v>46</v>
+      </c>
+      <c r="F6">
+        <v>787900</v>
       </c>
       <c r="G6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" t="s">
         <v>84</v>
       </c>
-      <c r="H6" t="s">
-        <v>91</v>
-      </c>
-      <c r="I6" t="s">
-        <v>91</v>
-      </c>
       <c r="J6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -928,28 +916,28 @@
         <v>2024</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" t="s">
-        <v>75</v>
+        <v>47</v>
+      </c>
+      <c r="F7">
+        <v>787010</v>
       </c>
       <c r="G7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="J7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -963,28 +951,28 @@
         <v>2024</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" t="s">
-        <v>77</v>
+        <v>48</v>
+      </c>
+      <c r="F8">
+        <v>787000</v>
       </c>
       <c r="G8" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J8" t="s">
+        <v>97</v>
+      </c>
+      <c r="K8" t="s">
         <v>102</v>
-      </c>
-      <c r="K8" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -998,28 +986,28 @@
         <v>2024</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" t="s">
-        <v>77</v>
+        <v>49</v>
+      </c>
+      <c r="F9">
+        <v>787000</v>
       </c>
       <c r="G9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H9" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I9" t="s">
+        <v>93</v>
+      </c>
+      <c r="J9" t="s">
+        <v>97</v>
+      </c>
+      <c r="K9" t="s">
         <v>98</v>
-      </c>
-      <c r="J9" t="s">
-        <v>102</v>
-      </c>
-      <c r="K9" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1033,28 +1021,28 @@
         <v>2024</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>787400</v>
+      </c>
+      <c r="G10" t="s">
         <v>79</v>
       </c>
-      <c r="G10" t="s">
-        <v>85</v>
-      </c>
       <c r="H10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="I10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J10" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1068,28 +1056,28 @@
         <v>2024</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" t="s">
-        <v>77</v>
+        <v>51</v>
+      </c>
+      <c r="F11">
+        <v>787000</v>
       </c>
       <c r="G11" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H11" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J11" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K11" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1103,28 +1091,28 @@
         <v>2024</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" t="s">
-        <v>75</v>
+        <v>52</v>
+      </c>
+      <c r="F12">
+        <v>787010</v>
       </c>
       <c r="G12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="J12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1138,63 +1126,63 @@
         <v>2024</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" t="s">
-        <v>78</v>
+        <v>53</v>
+      </c>
+      <c r="F13">
+        <v>787200</v>
       </c>
       <c r="G13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" t="s">
         <v>84</v>
       </c>
-      <c r="H13" t="s">
-        <v>91</v>
-      </c>
       <c r="I13" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="J13" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>17</v>
+      <c r="B14">
+        <v>9</v>
       </c>
       <c r="C14">
         <v>2024</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" t="s">
-        <v>76</v>
+        <v>54</v>
+      </c>
+      <c r="F14">
+        <v>787310</v>
       </c>
       <c r="G14" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H14" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I14" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="J14" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1208,28 +1196,28 @@
         <v>2024</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" t="s">
-        <v>77</v>
+        <v>55</v>
+      </c>
+      <c r="F15">
+        <v>787000</v>
       </c>
       <c r="G15" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H15" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I15" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J15" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1243,28 +1231,28 @@
         <v>2024</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16">
+        <v>787320</v>
+      </c>
+      <c r="G16" t="s">
         <v>80</v>
       </c>
-      <c r="G16" t="s">
-        <v>86</v>
-      </c>
       <c r="H16" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="I16" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="J16" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1278,28 +1266,28 @@
         <v>2024</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" t="s">
-        <v>77</v>
+        <v>57</v>
+      </c>
+      <c r="F17">
+        <v>787000</v>
       </c>
       <c r="G17" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H17" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I17" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J17" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K17" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1313,28 +1301,28 @@
         <v>2024</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" t="s">
-        <v>77</v>
+        <v>58</v>
+      </c>
+      <c r="F18">
+        <v>787000</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H18" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I18" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J18" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1348,28 +1336,28 @@
         <v>2024</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" t="s">
-        <v>77</v>
+        <v>59</v>
+      </c>
+      <c r="F19">
+        <v>787000</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H19" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I19" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1383,28 +1371,28 @@
         <v>2024</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" t="s">
-        <v>77</v>
+        <v>60</v>
+      </c>
+      <c r="F20">
+        <v>787000</v>
       </c>
       <c r="G20" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H20" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I20" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J20" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1418,28 +1406,28 @@
         <v>2024</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" t="s">
-        <v>77</v>
+        <v>61</v>
+      </c>
+      <c r="F21">
+        <v>787000</v>
       </c>
       <c r="G21" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H21" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I21" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J21" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K21" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1453,28 +1441,28 @@
         <v>2024</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" t="s">
-        <v>77</v>
+        <v>62</v>
+      </c>
+      <c r="F22">
+        <v>787000</v>
       </c>
       <c r="G22" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H22" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I22" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J22" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1488,28 +1476,28 @@
         <v>2024</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" t="s">
-        <v>77</v>
+        <v>63</v>
+      </c>
+      <c r="F23">
+        <v>787000</v>
       </c>
       <c r="G23" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H23" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I23" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J23" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K23" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1523,28 +1511,28 @@
         <v>2024</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E24" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24">
+        <v>787400</v>
+      </c>
+      <c r="G24" t="s">
         <v>79</v>
       </c>
-      <c r="G24" t="s">
-        <v>85</v>
-      </c>
       <c r="H24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="I24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="J24" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K24" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1558,28 +1546,28 @@
         <v>2024</v>
       </c>
       <c r="D25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" t="s">
-        <v>77</v>
+        <v>65</v>
+      </c>
+      <c r="F25">
+        <v>787000</v>
       </c>
       <c r="G25" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H25" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I25" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J25" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1593,28 +1581,28 @@
         <v>2023</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" t="s">
-        <v>75</v>
+        <v>66</v>
+      </c>
+      <c r="F26">
+        <v>787010</v>
       </c>
       <c r="G26" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H26" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I26" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="J26" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K26" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1628,28 +1616,28 @@
         <v>2023</v>
       </c>
       <c r="D27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E27" t="s">
-        <v>68</v>
-      </c>
-      <c r="F27" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="F27">
+        <v>787310</v>
       </c>
       <c r="G27" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H27" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I27" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="J27" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1663,28 +1651,28 @@
         <v>2023</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E28" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" t="s">
-        <v>77</v>
+        <v>68</v>
+      </c>
+      <c r="F28">
+        <v>787000</v>
       </c>
       <c r="G28" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H28" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I28" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J28" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K28" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1698,28 +1686,28 @@
         <v>2023</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E29" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" t="s">
-        <v>78</v>
+        <v>69</v>
+      </c>
+      <c r="F29">
+        <v>787000</v>
       </c>
       <c r="G29" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" t="s">
+        <v>82</v>
+      </c>
+      <c r="I29" t="s">
         <v>84</v>
       </c>
-      <c r="H29" t="s">
-        <v>91</v>
-      </c>
-      <c r="I29" t="s">
-        <v>91</v>
-      </c>
       <c r="J29" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1733,28 +1721,28 @@
         <v>2024</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F30" t="s">
-        <v>78</v>
+        <v>70</v>
+      </c>
+      <c r="F30">
+        <v>787200</v>
       </c>
       <c r="G30" t="s">
+        <v>76</v>
+      </c>
+      <c r="H30" t="s">
         <v>84</v>
       </c>
-      <c r="H30" t="s">
-        <v>91</v>
-      </c>
       <c r="I30" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="J30" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K30" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1768,28 +1756,28 @@
         <v>2024</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>72</v>
-      </c>
-      <c r="F31" t="s">
-        <v>75</v>
+        <v>71</v>
+      </c>
+      <c r="F31">
+        <v>787010</v>
       </c>
       <c r="G31" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H31" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I31" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="J31" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K31" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1803,28 +1791,28 @@
         <v>2024</v>
       </c>
       <c r="D32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F32" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="F32">
+        <v>787000</v>
       </c>
       <c r="G32" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H32" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I32" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J32" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1838,28 +1826,28 @@
         <v>2024</v>
       </c>
       <c r="D33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33">
+        <v>787000</v>
+      </c>
+      <c r="G33" t="s">
         <v>74</v>
       </c>
-      <c r="F33" t="s">
-        <v>77</v>
-      </c>
-      <c r="G33" t="s">
-        <v>83</v>
-      </c>
       <c r="H33" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I33" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J33" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K33" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1873,28 +1861,28 @@
         <v>2024</v>
       </c>
       <c r="D34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E34" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34">
+        <v>787900</v>
+      </c>
+      <c r="G34" t="s">
         <v>77</v>
       </c>
-      <c r="G34" t="s">
-        <v>83</v>
-      </c>
       <c r="H34" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I34" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J34" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K34" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1908,28 +1896,28 @@
         <v>2024</v>
       </c>
       <c r="D35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
-      </c>
-      <c r="F35" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35">
+        <v>787900</v>
+      </c>
+      <c r="G35" t="s">
         <v>77</v>
       </c>
-      <c r="G35" t="s">
-        <v>83</v>
-      </c>
       <c r="H35" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I35" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J35" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K35" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1943,19 +1931,45 @@
         <v>2024</v>
       </c>
       <c r="D36" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" t="s">
-        <v>77</v>
+        <v>41</v>
+      </c>
+      <c r="F36">
+        <v>787000</v>
       </c>
       <c r="G36" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H36" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="K36" t="s">
-        <v>106</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <v>22</v>
+      </c>
+      <c r="C37">
+        <v>2024</v>
+      </c>
+      <c r="D37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37">
+        <v>787000</v>
+      </c>
+      <c r="G37" t="s">
+        <v>74</v>
+      </c>
+      <c r="H37" t="s">
+        <v>82</v>
+      </c>
+      <c r="K37" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>